<commit_message>
excel sheet fix with hours
</commit_message>
<xml_diff>
--- a/assets/seedleResources.xlsx
+++ b/assets/seedleResources.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4209" uniqueCount="2200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4257" uniqueCount="2200">
   <si>
     <t>Province</t>
   </si>
@@ -4894,6 +4894,9 @@
     <t>https://www.webelievesurvivors.ca</t>
   </si>
   <si>
+    <t>24/7</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -5210,7 +5213,7 @@
     <t>Queen’s First Aid</t>
   </si>
   <si>
-    <t>Student-run first-aid and emergency response service available 24/7 during the academic year for on-campus medical emergencies.</t>
+    <t>Student-run first-aid and emergency response service always available during the academic year for on-campus medical emergencies.</t>
   </si>
   <si>
     <t>(613) 533-6111</t>
@@ -5236,9 +5239,6 @@
     </r>
   </si>
   <si>
-    <t>24/7 (during academic year)</t>
-  </si>
-  <si>
     <t>Engineering Mental Health Steward Program</t>
   </si>
   <si>
@@ -6187,7 +6187,7 @@
     <t>Campus Security</t>
   </si>
   <si>
-    <t>Campus security and emergency response for Queen’s University community. Emergency services available 24/7, non-emergency inquiries supported during regular hours.</t>
+    <t>Campus security and emergency response for Queen’s University community. Emergency services always available, non-emergency inquiries supported during regular hours.</t>
   </si>
   <si>
     <t>Emergency: (613)-533-6111; Non-emergency: (613)-533-6080; General: (613)-533-6733</t>
@@ -6197,9 +6197,6 @@
   </si>
   <si>
     <t>queensu.ca/risk/security</t>
-  </si>
-  <si>
-    <t>24/7 emergency response with non-emergency support during regular hours</t>
   </si>
   <si>
     <t>Unit 101, 1006 Princess Street, Kingston, ON K7L 1H2</t>
@@ -6804,6 +6801,9 @@
     <t>https://www.ontario.ca/page/get-medical-advice-telehealth-ontario</t>
   </si>
   <si>
+    <t xml:space="preserve"> '24/7</t>
+  </si>
+  <si>
     <t>TransFamily Kingston</t>
   </si>
   <si>
@@ -6920,10 +6920,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/m"/>
-  </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7024,6 +7021,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF212121"/>
       <name val="Arial"/>
@@ -7083,7 +7085,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7157,13 +7159,16 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -7199,7 +7204,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -7217,20 +7222,20 @@
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -39336,8 +39341,8 @@
       <c r="I13" s="22" t="s">
         <v>1588</v>
       </c>
-      <c r="J13" s="25">
-        <v>45862.0</v>
+      <c r="J13" s="25" t="s">
+        <v>1589</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>1510</v>
@@ -39348,7 +39353,7 @@
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -39370,28 +39375,28 @@
         <v>1501</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>1512</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>1549</v>
@@ -39428,25 +39433,25 @@
         <v>1501</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>1535</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="J15" s="24" t="s">
         <v>1568</v>
@@ -39486,25 +39491,25 @@
         <v>1501</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>1577</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>1583</v>
@@ -39544,25 +39549,25 @@
         <v>1501</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>1527</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>1583</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>1583</v>
@@ -39602,25 +39607,25 @@
         <v>1501</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>1535</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>1583</v>
@@ -39660,28 +39665,28 @@
         <v>1501</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>1549</v>
@@ -39718,28 +39723,28 @@
         <v>1501</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>1512</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>1580</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>1510</v>
@@ -39776,25 +39781,25 @@
         <v>1501</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>1527</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>1568</v>
@@ -39834,28 +39839,28 @@
         <v>1501</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>1510</v>
@@ -39892,25 +39897,25 @@
         <v>1501</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>1584</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>1525</v>
@@ -39950,28 +39955,28 @@
         <v>1501</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>1660</v>
-      </c>
-      <c r="J24" s="5" t="s">
         <v>1661</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>1589</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>1510</v>
@@ -40044,7 +40049,7 @@
         <v>1583</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -40102,7 +40107,7 @@
         <v>1583</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -40185,7 +40190,7 @@
         <v>1678</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>1679</v>
@@ -40321,10 +40326,10 @@
       <c r="J30" s="5" t="s">
         <v>1583</v>
       </c>
-      <c r="K30" s="28" t="s">
+      <c r="K30" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L30" s="28" t="s">
+      <c r="L30" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M30" s="9">
@@ -40379,10 +40384,10 @@
       <c r="J31" s="5" t="s">
         <v>1583</v>
       </c>
-      <c r="K31" s="28" t="s">
+      <c r="K31" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L31" s="28" t="s">
+      <c r="L31" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M31" s="9">
@@ -40437,10 +40442,10 @@
       <c r="J32" s="5" t="s">
         <v>1583</v>
       </c>
-      <c r="K32" s="28" t="s">
+      <c r="K32" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L32" s="28" t="s">
+      <c r="L32" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M32" s="9">
@@ -40465,34 +40470,34 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="29" t="s">
         <v>1392</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>1501</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="29" t="s">
         <v>1709</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>1503</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="29" t="s">
         <v>1710</v>
       </c>
-      <c r="F33" s="28" t="s">
+      <c r="F33" s="29" t="s">
         <v>1711</v>
       </c>
-      <c r="G33" s="28" t="s">
+      <c r="G33" s="29" t="s">
         <v>1712</v>
       </c>
-      <c r="H33" s="29" t="s">
+      <c r="H33" s="30" t="s">
         <v>1713</v>
       </c>
-      <c r="I33" s="30" t="s">
+      <c r="I33" s="31" t="s">
         <v>1714</v>
       </c>
-      <c r="J33" s="28" t="s">
+      <c r="J33" s="29" t="s">
         <v>1715</v>
       </c>
       <c r="K33" s="5" t="s">
@@ -40501,10 +40506,10 @@
       <c r="L33" s="5" t="s">
         <v>1510</v>
       </c>
-      <c r="M33" s="28">
+      <c r="M33" s="29">
         <v>44.22423</v>
       </c>
-      <c r="N33" s="28">
+      <c r="N33" s="29">
         <v>-76.4979</v>
       </c>
       <c r="O33" s="10" t="s">
@@ -40523,46 +40528,46 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="29" t="s">
         <v>1392</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="29" t="s">
         <v>1501</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="29" t="s">
         <v>1716</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>1641</v>
-      </c>
-      <c r="E34" s="28" t="s">
+        <v>1642</v>
+      </c>
+      <c r="E34" s="29" t="s">
         <v>1717</v>
       </c>
-      <c r="F34" s="28" t="s">
+      <c r="F34" s="29" t="s">
         <v>1718</v>
       </c>
-      <c r="G34" s="28" t="s">
+      <c r="G34" s="29" t="s">
         <v>1719</v>
       </c>
-      <c r="H34" s="29" t="s">
+      <c r="H34" s="30" t="s">
         <v>1720</v>
       </c>
-      <c r="I34" s="31" t="s">
+      <c r="I34" s="32" t="s">
         <v>1721</v>
       </c>
-      <c r="J34" s="28" t="s">
+      <c r="J34" s="29" t="s">
         <v>1722</v>
       </c>
-      <c r="K34" s="28" t="s">
+      <c r="K34" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L34" s="28" t="s">
+      <c r="L34" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="M34" s="28">
+      <c r="M34" s="29">
         <v>44.24003</v>
       </c>
-      <c r="N34" s="28">
+      <c r="N34" s="29">
         <v>-76.5088</v>
       </c>
       <c r="O34" s="10" t="s">
@@ -40581,46 +40586,46 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="29" t="s">
         <v>1392</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="29" t="s">
         <v>1501</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="29" t="s">
         <v>1723</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>1503</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="29" t="s">
         <v>1724</v>
       </c>
-      <c r="F35" s="28" t="s">
+      <c r="F35" s="29" t="s">
         <v>1725</v>
       </c>
-      <c r="G35" s="28" t="s">
+      <c r="G35" s="29" t="s">
         <v>1726</v>
       </c>
-      <c r="H35" s="29" t="s">
+      <c r="H35" s="30" t="s">
         <v>1727</v>
       </c>
-      <c r="I35" s="30" t="s">
+      <c r="I35" s="31" t="s">
         <v>1728</v>
       </c>
-      <c r="J35" s="28" t="s">
+      <c r="J35" s="29" t="s">
         <v>1729</v>
       </c>
-      <c r="K35" s="28" t="s">
+      <c r="K35" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L35" s="28" t="s">
+      <c r="L35" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="M35" s="28">
+      <c r="M35" s="29">
         <v>44.22485</v>
       </c>
-      <c r="N35" s="28">
+      <c r="N35" s="29">
         <v>-76.4968</v>
       </c>
       <c r="O35" s="10" t="s">
@@ -40639,46 +40644,46 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="29" t="s">
         <v>1392</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="29" t="s">
         <v>1501</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="29" t="s">
         <v>1730</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>1672</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="29" t="s">
         <v>1731</v>
       </c>
-      <c r="F36" s="28" t="s">
+      <c r="F36" s="29" t="s">
         <v>1732</v>
       </c>
-      <c r="G36" s="28" t="s">
+      <c r="G36" s="29" t="s">
         <v>1733</v>
       </c>
-      <c r="H36" s="32" t="s">
+      <c r="H36" s="33" t="s">
         <v>1734</v>
       </c>
-      <c r="I36" s="30" t="s">
+      <c r="I36" s="31" t="s">
         <v>1735</v>
       </c>
-      <c r="J36" s="28" t="s">
+      <c r="J36" s="29" t="s">
         <v>1736</v>
       </c>
-      <c r="K36" s="28" t="s">
+      <c r="K36" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L36" s="28" t="s">
+      <c r="L36" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="M36" s="28">
+      <c r="M36" s="29">
         <v>44.23729</v>
       </c>
-      <c r="N36" s="28">
+      <c r="N36" s="29">
         <v>-76.5012</v>
       </c>
       <c r="O36" s="10" t="s">
@@ -40697,46 +40702,46 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="29" t="s">
         <v>1392</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="29" t="s">
         <v>1501</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="29" t="s">
         <v>1737</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>1738</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="29" t="s">
         <v>1739</v>
       </c>
-      <c r="F37" s="28" t="s">
+      <c r="F37" s="29" t="s">
         <v>1740</v>
       </c>
-      <c r="G37" s="28" t="s">
+      <c r="G37" s="29" t="s">
         <v>1741</v>
       </c>
-      <c r="H37" s="29" t="s">
+      <c r="H37" s="30" t="s">
         <v>1742</v>
       </c>
-      <c r="I37" s="30" t="s">
+      <c r="I37" s="31" t="s">
         <v>1743</v>
       </c>
-      <c r="J37" s="28" t="s">
+      <c r="J37" s="29" t="s">
         <v>1744</v>
       </c>
-      <c r="K37" s="28" t="s">
+      <c r="K37" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L37" s="28" t="s">
+      <c r="L37" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="M37" s="28">
+      <c r="M37" s="29">
         <v>44.22735</v>
       </c>
-      <c r="N37" s="28">
+      <c r="N37" s="29">
         <v>-76.4909</v>
       </c>
       <c r="O37" s="10" t="s">
@@ -40755,10 +40760,10 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="29" t="s">
         <v>1392</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C38" s="17" t="s">
@@ -40767,19 +40772,19 @@
       <c r="D38" s="10" t="s">
         <v>1512</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="29" t="s">
         <v>1746</v>
       </c>
-      <c r="F38" s="28" t="s">
+      <c r="F38" s="29" t="s">
         <v>1747</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="H38" s="29" t="s">
+      <c r="H38" s="30" t="s">
         <v>1748</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I38" s="34" t="s">
         <v>1749</v>
       </c>
       <c r="J38" s="17" t="s">
@@ -40837,16 +40842,16 @@
       <c r="H39" s="27" t="s">
         <v>1755</v>
       </c>
-      <c r="I39" s="34" t="s">
+      <c r="I39" s="35" t="s">
         <v>1756</v>
       </c>
-      <c r="J39" s="35" t="s">
+      <c r="J39" s="36" t="s">
         <v>1757</v>
       </c>
-      <c r="K39" s="36" t="s">
+      <c r="K39" s="37" t="s">
         <v>1510</v>
       </c>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="37" t="s">
         <v>1510</v>
       </c>
       <c r="M39" s="9">
@@ -40874,7 +40879,7 @@
       <c r="A40" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C40" s="17" t="s">
@@ -40892,19 +40897,19 @@
       <c r="G40" s="17" t="s">
         <v>1761</v>
       </c>
-      <c r="H40" s="29" t="s">
+      <c r="H40" s="30" t="s">
         <v>1762</v>
       </c>
-      <c r="I40" s="31" t="s">
+      <c r="I40" s="32" t="s">
         <v>1763</v>
       </c>
       <c r="J40" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="K40" s="37" t="s">
+      <c r="K40" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L40" s="37" t="s">
+      <c r="L40" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M40" s="17">
@@ -40932,7 +40937,7 @@
       <c r="A41" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C41" s="17" t="s">
@@ -40950,19 +40955,19 @@
       <c r="G41" s="17" t="s">
         <v>1767</v>
       </c>
-      <c r="H41" s="29" t="s">
+      <c r="H41" s="30" t="s">
         <v>1768</v>
       </c>
-      <c r="I41" s="31" t="s">
+      <c r="I41" s="32" t="s">
         <v>1769</v>
       </c>
       <c r="J41" s="17" t="s">
         <v>1770</v>
       </c>
-      <c r="K41" s="37" t="s">
+      <c r="K41" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L41" s="37" t="s">
+      <c r="L41" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M41" s="17">
@@ -40990,7 +40995,7 @@
       <c r="A42" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C42" s="17" t="s">
@@ -41008,19 +41013,19 @@
       <c r="G42" s="17" t="s">
         <v>1774</v>
       </c>
-      <c r="H42" s="29" t="s">
+      <c r="H42" s="30" t="s">
         <v>1775</v>
       </c>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="32" t="s">
         <v>1776</v>
       </c>
       <c r="J42" s="17" t="s">
         <v>1777</v>
       </c>
-      <c r="K42" s="37" t="s">
+      <c r="K42" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L42" s="37" t="s">
+      <c r="L42" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M42" s="17">
@@ -41048,7 +41053,7 @@
       <c r="A43" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C43" s="17" t="s">
@@ -41066,19 +41071,19 @@
       <c r="G43" s="17" t="s">
         <v>1781</v>
       </c>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="31" t="s">
         <v>1782</v>
       </c>
-      <c r="I43" s="31" t="s">
+      <c r="I43" s="32" t="s">
         <v>1783</v>
       </c>
       <c r="J43" s="17" t="s">
         <v>1784</v>
       </c>
-      <c r="K43" s="38" t="s">
+      <c r="K43" s="39" t="s">
         <v>1549</v>
       </c>
-      <c r="L43" s="38" t="s">
+      <c r="L43" s="39" t="s">
         <v>1549</v>
       </c>
       <c r="M43" s="17">
@@ -41106,14 +41111,14 @@
       <c r="A44" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>1785</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>1786</v>
@@ -41124,7 +41129,7 @@
       <c r="G44" s="5" t="s">
         <v>1788</v>
       </c>
-      <c r="H44" s="29" t="s">
+      <c r="H44" s="30" t="s">
         <v>1789</v>
       </c>
       <c r="I44" s="21" t="s">
@@ -41133,10 +41138,10 @@
       <c r="J44" s="5" t="s">
         <v>1583</v>
       </c>
-      <c r="K44" s="37" t="s">
+      <c r="K44" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L44" s="37" t="s">
+      <c r="L44" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M44" s="17">
@@ -41164,14 +41169,14 @@
       <c r="A45" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>1791</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>1792</v>
@@ -41182,19 +41187,19 @@
       <c r="G45" s="5" t="s">
         <v>1794</v>
       </c>
-      <c r="H45" s="29" t="s">
+      <c r="H45" s="30" t="s">
         <v>1795</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>1796</v>
       </c>
-      <c r="J45" s="39">
-        <v>45862.0</v>
-      </c>
-      <c r="K45" s="37" t="s">
+      <c r="J45" s="40" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K45" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L45" s="37" t="s">
+      <c r="L45" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M45" s="17">
@@ -41222,7 +41227,7 @@
       <c r="A46" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C46" s="17" t="s">
@@ -41240,19 +41245,19 @@
       <c r="G46" s="5" t="s">
         <v>1800</v>
       </c>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="30" t="s">
         <v>1801</v>
       </c>
       <c r="I46" s="21" t="s">
         <v>1802</v>
       </c>
-      <c r="J46" s="39">
-        <v>45862.0</v>
-      </c>
-      <c r="K46" s="37" t="s">
+      <c r="J46" s="40" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K46" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L46" s="37" t="s">
+      <c r="L46" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M46" s="17">
@@ -41298,19 +41303,19 @@
       <c r="G47" s="5" t="s">
         <v>1807</v>
       </c>
-      <c r="H47" s="40" t="s">
+      <c r="H47" s="41" t="s">
         <v>1808</v>
       </c>
       <c r="I47" s="22" t="s">
         <v>1809</v>
       </c>
-      <c r="J47" s="39">
-        <v>45862.0</v>
-      </c>
-      <c r="K47" s="37" t="s">
+      <c r="J47" s="40" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K47" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L47" s="37" t="s">
+      <c r="L47" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M47" s="17">
@@ -41338,7 +41343,7 @@
       <c r="A48" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B48" s="28" t="s">
+      <c r="B48" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C48" s="17" t="s">
@@ -41356,7 +41361,7 @@
       <c r="G48" s="5" t="s">
         <v>1813</v>
       </c>
-      <c r="H48" s="29" t="s">
+      <c r="H48" s="30" t="s">
         <v>1814</v>
       </c>
       <c r="I48" s="21" t="s">
@@ -41365,10 +41370,10 @@
       <c r="J48" s="5" t="s">
         <v>1816</v>
       </c>
-      <c r="K48" s="37" t="s">
+      <c r="K48" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L48" s="37" t="s">
+      <c r="L48" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M48" s="17">
@@ -41396,7 +41401,7 @@
       <c r="A49" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C49" s="17" t="s">
@@ -41414,19 +41419,19 @@
       <c r="G49" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="H49" s="30" t="s">
+      <c r="H49" s="31" t="s">
         <v>1820</v>
       </c>
-      <c r="I49" s="33" t="s">
+      <c r="I49" s="34" t="s">
         <v>1821</v>
       </c>
       <c r="J49" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="K49" s="37" t="s">
+      <c r="K49" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L49" s="37" t="s">
+      <c r="L49" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M49" s="17">
@@ -41454,7 +41459,7 @@
       <c r="A50" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C50" s="17" t="s">
@@ -41472,19 +41477,19 @@
       <c r="G50" s="17" t="s">
         <v>1826</v>
       </c>
-      <c r="H50" s="29" t="s">
+      <c r="H50" s="30" t="s">
         <v>1827</v>
       </c>
-      <c r="I50" s="31" t="s">
+      <c r="I50" s="32" t="s">
         <v>1828</v>
       </c>
       <c r="J50" s="17" t="s">
         <v>1829</v>
       </c>
-      <c r="K50" s="37" t="s">
+      <c r="K50" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L50" s="37" t="s">
+      <c r="L50" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M50" s="17">
@@ -41512,7 +41517,7 @@
       <c r="A51" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C51" s="17" t="s">
@@ -41530,19 +41535,19 @@
       <c r="G51" s="5" t="s">
         <v>1833</v>
       </c>
-      <c r="H51" s="29" t="s">
+      <c r="H51" s="30" t="s">
         <v>1834</v>
       </c>
       <c r="I51" s="22" t="s">
         <v>1835</v>
       </c>
-      <c r="J51" s="41" t="s">
+      <c r="J51" s="42" t="s">
         <v>1836</v>
       </c>
-      <c r="K51" s="37" t="s">
+      <c r="K51" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L51" s="37" t="s">
+      <c r="L51" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M51" s="17">
@@ -41570,7 +41575,7 @@
       <c r="A52" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C52" s="17" t="s">
@@ -41588,7 +41593,7 @@
       <c r="G52" s="5" t="s">
         <v>1840</v>
       </c>
-      <c r="H52" s="29" t="s">
+      <c r="H52" s="30" t="s">
         <v>1814</v>
       </c>
       <c r="I52" s="22" t="s">
@@ -41597,10 +41602,10 @@
       <c r="J52" s="5" t="s">
         <v>1842</v>
       </c>
-      <c r="K52" s="37" t="s">
+      <c r="K52" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L52" s="37" t="s">
+      <c r="L52" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M52" s="17">
@@ -41628,7 +41633,7 @@
       <c r="A53" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C53" s="17" t="s">
@@ -41646,19 +41651,19 @@
       <c r="G53" s="5" t="s">
         <v>1833</v>
       </c>
-      <c r="H53" s="29" t="s">
+      <c r="H53" s="30" t="s">
         <v>1834</v>
       </c>
       <c r="I53" s="22" t="s">
         <v>1845</v>
       </c>
-      <c r="J53" s="39">
-        <v>45862.0</v>
-      </c>
-      <c r="K53" s="37" t="s">
+      <c r="J53" s="40" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K53" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L53" s="37" t="s">
+      <c r="L53" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M53" s="17">
@@ -41686,7 +41691,7 @@
       <c r="A54" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C54" s="17" t="s">
@@ -41704,7 +41709,7 @@
       <c r="G54" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="H54" s="40" t="s">
+      <c r="H54" s="41" t="s">
         <v>1849</v>
       </c>
       <c r="I54" s="21" t="s">
@@ -41713,10 +41718,10 @@
       <c r="J54" s="17" t="s">
         <v>1829</v>
       </c>
-      <c r="K54" s="37" t="s">
+      <c r="K54" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L54" s="37" t="s">
+      <c r="L54" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M54" s="17">
@@ -41744,7 +41749,7 @@
       <c r="A55" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C55" s="17" t="s">
@@ -41762,7 +41767,7 @@
       <c r="G55" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="H55" s="29" t="s">
+      <c r="H55" s="30" t="s">
         <v>1854</v>
       </c>
       <c r="I55" s="22" t="s">
@@ -41771,10 +41776,10 @@
       <c r="J55" s="5" t="s">
         <v>1856</v>
       </c>
-      <c r="K55" s="37" t="s">
+      <c r="K55" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L55" s="37" t="s">
+      <c r="L55" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M55" s="17">
@@ -41802,7 +41807,7 @@
       <c r="A56" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C56" s="17" t="s">
@@ -41823,16 +41828,16 @@
       <c r="H56" s="17" t="s">
         <v>1720</v>
       </c>
-      <c r="I56" s="33" t="s">
+      <c r="I56" s="34" t="s">
         <v>1860</v>
       </c>
       <c r="J56" s="17" t="s">
         <v>1861</v>
       </c>
-      <c r="K56" s="37" t="s">
+      <c r="K56" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L56" s="37" t="s">
+      <c r="L56" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M56" s="17">
@@ -41860,7 +41865,7 @@
       <c r="A57" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C57" s="17" t="s">
@@ -41881,16 +41886,16 @@
       <c r="H57" s="17" t="s">
         <v>1866</v>
       </c>
-      <c r="I57" s="42" t="s">
+      <c r="I57" s="43" t="s">
         <v>1867</v>
       </c>
       <c r="J57" s="17" t="s">
         <v>1868</v>
       </c>
-      <c r="K57" s="38" t="s">
+      <c r="K57" s="39" t="s">
         <v>1869</v>
       </c>
-      <c r="L57" s="38" t="s">
+      <c r="L57" s="39" t="s">
         <v>1869</v>
       </c>
       <c r="M57" s="17">
@@ -41918,7 +41923,7 @@
       <c r="A58" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C58" s="17" t="s">
@@ -41939,16 +41944,16 @@
       <c r="H58" s="17" t="s">
         <v>1874</v>
       </c>
-      <c r="I58" s="33" t="s">
+      <c r="I58" s="34" t="s">
         <v>1875</v>
       </c>
       <c r="J58" s="17" t="s">
         <v>1876</v>
       </c>
-      <c r="K58" s="37" t="s">
+      <c r="K58" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L58" s="37" t="s">
+      <c r="L58" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M58" s="17">
@@ -41976,7 +41981,7 @@
       <c r="A59" s="17" t="s">
         <v>1392</v>
       </c>
-      <c r="B59" s="28" t="s">
+      <c r="B59" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C59" s="17" t="s">
@@ -41997,16 +42002,16 @@
       <c r="H59" s="17" t="s">
         <v>1881</v>
       </c>
-      <c r="I59" s="42" t="s">
+      <c r="I59" s="43" t="s">
         <v>1828</v>
       </c>
       <c r="J59" s="17" t="s">
         <v>1882</v>
       </c>
-      <c r="K59" s="37" t="s">
+      <c r="K59" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L59" s="37" t="s">
+      <c r="L59" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M59" s="17">
@@ -42031,10 +42036,10 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60">
-      <c r="A60" s="43" t="s">
+      <c r="A60" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="44" t="s">
         <v>1501</v>
       </c>
       <c r="C60" s="17" t="s">
@@ -42055,16 +42060,16 @@
       <c r="H60" s="17" t="s">
         <v>1887</v>
       </c>
-      <c r="I60" s="42" t="s">
+      <c r="I60" s="43" t="s">
         <v>1582</v>
       </c>
       <c r="J60" s="17" t="s">
         <v>1888</v>
       </c>
-      <c r="K60" s="37" t="s">
+      <c r="K60" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L60" s="37" t="s">
+      <c r="L60" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M60" s="17">
@@ -42089,10 +42094,10 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61">
-      <c r="A61" s="43" t="s">
+      <c r="A61" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="B61" s="43" t="s">
+      <c r="B61" s="44" t="s">
         <v>1501</v>
       </c>
       <c r="C61" s="17" t="s">
@@ -42113,16 +42118,16 @@
       <c r="H61" s="17" t="s">
         <v>1893</v>
       </c>
-      <c r="I61" s="42" t="s">
+      <c r="I61" s="43" t="s">
         <v>1894</v>
       </c>
       <c r="J61" s="17" t="s">
         <v>1895</v>
       </c>
-      <c r="K61" s="37" t="s">
+      <c r="K61" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L61" s="37" t="s">
+      <c r="L61" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M61" s="17">
@@ -42147,10 +42152,10 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="44" t="s">
         <v>1501</v>
       </c>
       <c r="C62" s="17" t="s">
@@ -42171,22 +42176,22 @@
       <c r="H62" s="17" t="s">
         <v>1900</v>
       </c>
-      <c r="I62" s="33" t="s">
+      <c r="I62" s="34" t="s">
         <v>1901</v>
       </c>
       <c r="J62" s="17" t="s">
         <v>1902</v>
       </c>
-      <c r="K62" s="37" t="s">
+      <c r="K62" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L62" s="37" t="s">
+      <c r="L62" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="M62" s="44">
+      <c r="M62" s="45">
         <v>44.2272764753702</v>
       </c>
-      <c r="N62" s="44">
+      <c r="N62" s="45">
         <v>-76.4967588846576</v>
       </c>
       <c r="O62" s="10" t="s">
@@ -42205,10 +42210,10 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="44" t="s">
         <v>1501</v>
       </c>
       <c r="C63" s="17" t="s">
@@ -42229,16 +42234,16 @@
       <c r="H63" s="17" t="s">
         <v>1907</v>
       </c>
-      <c r="I63" s="33" t="s">
+      <c r="I63" s="34" t="s">
         <v>1908</v>
       </c>
       <c r="J63" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="K63" s="37" t="s">
+      <c r="K63" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L63" s="37" t="s">
+      <c r="L63" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M63" s="17">
@@ -42263,10 +42268,10 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64">
-      <c r="A64" s="43" t="s">
+      <c r="A64" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="B64" s="43" t="s">
+      <c r="B64" s="44" t="s">
         <v>1501</v>
       </c>
       <c r="C64" s="17" t="s">
@@ -42287,16 +42292,16 @@
       <c r="H64" s="17" t="s">
         <v>1913</v>
       </c>
-      <c r="I64" s="33" t="s">
+      <c r="I64" s="34" t="s">
         <v>1914</v>
       </c>
       <c r="J64" s="17" t="s">
         <v>1915</v>
       </c>
-      <c r="K64" s="37" t="s">
+      <c r="K64" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L64" s="37" t="s">
+      <c r="L64" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M64" s="17">
@@ -42321,10 +42326,10 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="44" t="s">
         <v>1501</v>
       </c>
       <c r="C65" s="17" t="s">
@@ -42345,16 +42350,16 @@
       <c r="H65" s="17" t="s">
         <v>1920</v>
       </c>
-      <c r="I65" s="33" t="s">
+      <c r="I65" s="34" t="s">
         <v>1921</v>
       </c>
       <c r="J65" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="K65" s="37" t="s">
+      <c r="K65" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L65" s="37" t="s">
+      <c r="L65" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M65" s="17">
@@ -42379,10 +42384,10 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66">
-      <c r="A66" s="43" t="s">
+      <c r="A66" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="44" t="s">
         <v>1501</v>
       </c>
       <c r="C66" s="17" t="s">
@@ -42403,16 +42408,16 @@
       <c r="H66" s="17" t="s">
         <v>1926</v>
       </c>
-      <c r="I66" s="33" t="s">
+      <c r="I66" s="34" t="s">
         <v>1927</v>
       </c>
       <c r="J66" s="17" t="s">
         <v>1928</v>
       </c>
-      <c r="K66" s="37" t="s">
+      <c r="K66" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L66" s="37" t="s">
+      <c r="L66" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M66" s="17">
@@ -42437,10 +42442,10 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="44" t="s">
         <v>1392</v>
       </c>
-      <c r="B67" s="43" t="s">
+      <c r="B67" s="44" t="s">
         <v>1501</v>
       </c>
       <c r="C67" s="17" t="s">
@@ -42461,16 +42466,16 @@
       <c r="H67" s="17" t="s">
         <v>1933</v>
       </c>
-      <c r="I67" s="33" t="s">
+      <c r="I67" s="34" t="s">
         <v>1934</v>
       </c>
       <c r="J67" s="17" t="s">
         <v>1935</v>
       </c>
-      <c r="K67" s="37" t="s">
+      <c r="K67" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L67" s="37" t="s">
+      <c r="L67" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M67" s="17">
@@ -42495,7 +42500,7 @@
       <c r="Z67" s="2"/>
     </row>
     <row r="68">
-      <c r="A68" s="43" t="s">
+      <c r="A68" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B68" s="17" t="s">
@@ -42505,7 +42510,7 @@
         <v>1936</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="E68" s="17" t="s">
         <v>1937</v>
@@ -42519,7 +42524,7 @@
       <c r="H68" s="17" t="s">
         <v>1940</v>
       </c>
-      <c r="I68" s="42" t="s">
+      <c r="I68" s="43" t="s">
         <v>1941</v>
       </c>
       <c r="J68" s="17" t="s">
@@ -42528,7 +42533,7 @@
       <c r="K68" s="17" t="s">
         <v>1943</v>
       </c>
-      <c r="L68" s="37" t="s">
+      <c r="L68" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M68" s="17">
@@ -42553,7 +42558,7 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69">
-      <c r="A69" s="43" t="s">
+      <c r="A69" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B69" s="17" t="s">
@@ -42563,7 +42568,7 @@
         <v>1944</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>1945</v>
@@ -42577,16 +42582,16 @@
       <c r="H69" s="17" t="s">
         <v>1948</v>
       </c>
-      <c r="I69" s="42" t="s">
+      <c r="I69" s="43" t="s">
         <v>1949</v>
       </c>
       <c r="J69" s="17" t="s">
         <v>1950</v>
       </c>
-      <c r="K69" s="37" t="s">
+      <c r="K69" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L69" s="37" t="s">
+      <c r="L69" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M69" s="17">
@@ -42611,7 +42616,7 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70">
-      <c r="A70" s="43" t="s">
+      <c r="A70" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B70" s="17" t="s">
@@ -42635,16 +42640,16 @@
       <c r="H70" s="17" t="s">
         <v>1675</v>
       </c>
-      <c r="I70" s="33" t="s">
+      <c r="I70" s="34" t="s">
         <v>1955</v>
       </c>
       <c r="J70" s="17" t="s">
         <v>1888</v>
       </c>
-      <c r="K70" s="37" t="s">
+      <c r="K70" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L70" s="37" t="s">
+      <c r="L70" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M70" s="17">
@@ -42669,7 +42674,7 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B71" s="17" t="s">
@@ -42693,16 +42698,16 @@
       <c r="H71" s="17" t="s">
         <v>1675</v>
       </c>
-      <c r="I71" s="42" t="s">
+      <c r="I71" s="43" t="s">
         <v>1960</v>
       </c>
       <c r="J71" s="17" t="s">
         <v>1961</v>
       </c>
-      <c r="K71" s="37" t="s">
+      <c r="K71" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L71" s="37" t="s">
+      <c r="L71" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M71" s="17">
@@ -42727,7 +42732,7 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B72" s="17" t="s">
@@ -42737,7 +42742,7 @@
         <v>1962</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E72" s="17" t="s">
         <v>1963</v>
@@ -42751,16 +42756,16 @@
       <c r="H72" s="17" t="s">
         <v>1966</v>
       </c>
-      <c r="I72" s="33" t="s">
+      <c r="I72" s="34" t="s">
         <v>1967</v>
       </c>
-      <c r="J72" s="17" t="s">
-        <v>1968</v>
-      </c>
-      <c r="K72" s="37" t="s">
+      <c r="J72" s="46" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K72" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L72" s="37" t="s">
+      <c r="L72" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M72" s="17">
@@ -42785,40 +42790,40 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73">
-      <c r="A73" s="43" t="s">
+      <c r="A73" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B73" s="17" t="s">
         <v>1501</v>
       </c>
       <c r="C73" s="17" t="s">
+        <v>1968</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>1656</v>
+      </c>
+      <c r="E73" s="17" t="s">
         <v>1969</v>
       </c>
-      <c r="D73" s="10" t="s">
-        <v>1655</v>
-      </c>
-      <c r="E73" s="17" t="s">
+      <c r="F73" s="17" t="s">
         <v>1970</v>
       </c>
-      <c r="F73" s="17" t="s">
+      <c r="G73" s="17" t="s">
         <v>1971</v>
       </c>
-      <c r="G73" s="17" t="s">
+      <c r="H73" s="17" t="s">
         <v>1972</v>
       </c>
-      <c r="H73" s="17" t="s">
+      <c r="I73" s="43" t="s">
         <v>1973</v>
       </c>
-      <c r="I73" s="42" t="s">
+      <c r="J73" s="17" t="s">
         <v>1974</v>
       </c>
-      <c r="J73" s="17" t="s">
-        <v>1975</v>
-      </c>
-      <c r="K73" s="37" t="s">
+      <c r="K73" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L73" s="37" t="s">
+      <c r="L73" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M73" s="17">
@@ -42843,40 +42848,40 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74">
-      <c r="A74" s="43" t="s">
+      <c r="A74" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B74" s="17" t="s">
         <v>1501</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="D74" s="10" t="s">
         <v>1672</v>
       </c>
       <c r="E74" s="17" t="s">
+        <v>1976</v>
+      </c>
+      <c r="F74" s="17" t="s">
         <v>1977</v>
       </c>
-      <c r="F74" s="17" t="s">
+      <c r="G74" s="17" t="s">
         <v>1978</v>
       </c>
-      <c r="G74" s="17" t="s">
+      <c r="H74" s="17" t="s">
         <v>1979</v>
       </c>
-      <c r="H74" s="17" t="s">
+      <c r="I74" s="34" t="s">
         <v>1980</v>
       </c>
-      <c r="I74" s="33" t="s">
+      <c r="J74" s="17" t="s">
         <v>1981</v>
       </c>
-      <c r="J74" s="17" t="s">
-        <v>1982</v>
-      </c>
-      <c r="K74" s="37" t="s">
+      <c r="K74" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L74" s="37" t="s">
+      <c r="L74" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M74" s="17">
@@ -42901,14 +42906,14 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75">
-      <c r="A75" s="43" t="s">
+      <c r="A75" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B75" s="17" t="s">
         <v>1501</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="D75" s="10" t="s">
         <v>1535</v>
@@ -42917,24 +42922,24 @@
         <v>1536</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="G75" s="17" t="s">
         <v>1538</v>
       </c>
       <c r="H75" s="17" t="s">
+        <v>1984</v>
+      </c>
+      <c r="I75" s="43" t="s">
         <v>1985</v>
       </c>
-      <c r="I75" s="42" t="s">
+      <c r="J75" s="17" t="s">
         <v>1986</v>
       </c>
-      <c r="J75" s="17" t="s">
-        <v>1987</v>
-      </c>
-      <c r="K75" s="37" t="s">
+      <c r="K75" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L75" s="37" t="s">
+      <c r="L75" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M75" s="17">
@@ -42959,40 +42964,40 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76">
-      <c r="A76" s="43" t="s">
+      <c r="A76" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B76" s="17" t="s">
         <v>1501</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>1672</v>
       </c>
       <c r="E76" s="17" t="s">
+        <v>1988</v>
+      </c>
+      <c r="F76" s="17" t="s">
         <v>1989</v>
       </c>
-      <c r="F76" s="17" t="s">
+      <c r="G76" s="17" t="s">
         <v>1990</v>
       </c>
-      <c r="G76" s="17" t="s">
+      <c r="H76" s="17" t="s">
         <v>1991</v>
       </c>
-      <c r="H76" s="17" t="s">
+      <c r="I76" s="43" t="s">
         <v>1992</v>
       </c>
-      <c r="I76" s="42" t="s">
+      <c r="J76" s="17" t="s">
         <v>1993</v>
       </c>
-      <c r="J76" s="17" t="s">
-        <v>1994</v>
-      </c>
-      <c r="K76" s="37" t="s">
+      <c r="K76" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L76" s="37" t="s">
+      <c r="L76" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M76" s="17">
@@ -43017,40 +43022,40 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77">
-      <c r="A77" s="45" t="s">
+      <c r="A77" s="47" t="s">
         <v>1392</v>
       </c>
       <c r="B77" s="17" t="s">
         <v>1803</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>1672</v>
       </c>
       <c r="E77" s="17" t="s">
+        <v>1995</v>
+      </c>
+      <c r="F77" s="17" t="s">
         <v>1996</v>
       </c>
-      <c r="F77" s="17" t="s">
+      <c r="G77" s="17" t="s">
         <v>1997</v>
       </c>
-      <c r="G77" s="17" t="s">
+      <c r="H77" s="17" t="s">
         <v>1998</v>
       </c>
-      <c r="H77" s="17" t="s">
+      <c r="I77" s="43" t="s">
         <v>1999</v>
       </c>
-      <c r="I77" s="42" t="s">
-        <v>2000</v>
-      </c>
       <c r="J77" s="17" t="s">
-        <v>1994</v>
-      </c>
-      <c r="K77" s="37" t="s">
+        <v>1993</v>
+      </c>
+      <c r="K77" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L77" s="37" t="s">
+      <c r="L77" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M77" s="17">
@@ -43075,40 +43080,40 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78">
-      <c r="A78" s="45" t="s">
+      <c r="A78" s="47" t="s">
         <v>1392</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>1501</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>1527</v>
       </c>
       <c r="E78" s="17" t="s">
+        <v>2001</v>
+      </c>
+      <c r="F78" s="17" t="s">
         <v>2002</v>
       </c>
-      <c r="F78" s="17" t="s">
+      <c r="G78" s="17" t="s">
         <v>2003</v>
       </c>
-      <c r="G78" s="17" t="s">
+      <c r="H78" s="17" t="s">
         <v>2004</v>
       </c>
-      <c r="H78" s="17" t="s">
+      <c r="I78" s="34" t="s">
         <v>2005</v>
       </c>
-      <c r="I78" s="33" t="s">
+      <c r="J78" s="17" t="s">
         <v>2006</v>
       </c>
-      <c r="J78" s="17" t="s">
-        <v>2007</v>
-      </c>
-      <c r="K78" s="37" t="s">
+      <c r="K78" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L78" s="37" t="s">
+      <c r="L78" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M78" s="17">
@@ -43133,23 +43138,23 @@
       <c r="Z78" s="2"/>
     </row>
     <row r="79">
-      <c r="A79" s="45" t="s">
+      <c r="A79" s="47" t="s">
         <v>1392</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>1501</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>1503</v>
       </c>
       <c r="E79" s="17" t="s">
+        <v>2008</v>
+      </c>
+      <c r="F79" s="17" t="s">
         <v>2009</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>2010</v>
       </c>
       <c r="G79" s="17" t="s">
         <v>1506</v>
@@ -43157,16 +43162,16 @@
       <c r="H79" s="17" t="s">
         <v>1507</v>
       </c>
-      <c r="I79" s="33" t="s">
+      <c r="I79" s="34" t="s">
+        <v>2010</v>
+      </c>
+      <c r="J79" s="17" t="s">
         <v>2011</v>
       </c>
-      <c r="J79" s="17" t="s">
-        <v>2012</v>
-      </c>
-      <c r="K79" s="37" t="s">
+      <c r="K79" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L79" s="37" t="s">
+      <c r="L79" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M79" s="17">
@@ -43191,40 +43196,40 @@
       <c r="Z79" s="2"/>
     </row>
     <row r="80">
-      <c r="A80" s="43" t="s">
+      <c r="A80" s="44" t="s">
         <v>1392</v>
       </c>
       <c r="B80" s="17" t="s">
         <v>1501</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D80" s="10" t="s">
         <v>1503</v>
       </c>
       <c r="E80" s="17" t="s">
+        <v>2013</v>
+      </c>
+      <c r="F80" s="17" t="s">
         <v>2014</v>
       </c>
-      <c r="F80" s="17" t="s">
+      <c r="G80" s="17" t="s">
         <v>2015</v>
       </c>
-      <c r="G80" s="17" t="s">
+      <c r="H80" s="17" t="s">
         <v>2016</v>
       </c>
-      <c r="H80" s="17" t="s">
+      <c r="I80" s="43" t="s">
         <v>2017</v>
-      </c>
-      <c r="I80" s="42" t="s">
-        <v>2018</v>
       </c>
       <c r="J80" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="K80" s="37" t="s">
+      <c r="K80" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L80" s="37" t="s">
+      <c r="L80" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M80" s="17">
@@ -67737,8 +67742,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="48" t="s">
+        <v>1589</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -67794,25 +67799,25 @@
         <v>1583</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>1655</v>
-      </c>
-      <c r="E2" s="46" t="s">
+        <v>1656</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>2018</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>2019</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>2020</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>2021</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>2022</v>
-      </c>
-      <c r="J2" s="47">
-        <v>45862.0</v>
+        <v>2021</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>1589</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>1510</v>
@@ -67827,7 +67832,7 @@
         <v>1583</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="3">
@@ -67844,20 +67849,20 @@
         <v>1577</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>2022</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>2023</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>2024</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>2025</v>
-      </c>
-      <c r="J3" s="47">
-        <v>45862.0</v>
+        <v>2024</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>1589</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>1510</v>
@@ -67872,7 +67877,7 @@
         <v>1583</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P3" s="2"/>
     </row>
@@ -67887,25 +67892,25 @@
         <v>1583</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>2025</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>2026</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>2027</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>2028</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>2029</v>
-      </c>
-      <c r="J4" s="47">
-        <v>45862.0</v>
+        <v>2028</v>
+      </c>
+      <c r="J4" s="48" t="s">
+        <v>1589</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>1510</v>
@@ -67920,45 +67925,45 @@
         <v>1583</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>1392</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="29" t="s">
         <v>1501</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>1583</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>1655</v>
-      </c>
-      <c r="E5" s="28" t="s">
+        <v>1656</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>2029</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>2030</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="G5" s="29" t="s">
         <v>2031</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="H5" s="12" t="s">
         <v>2032</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="31" t="s">
         <v>2033</v>
       </c>
-      <c r="I5" s="30" t="s">
-        <v>2034</v>
-      </c>
-      <c r="J5" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K5" s="28" t="s">
+      <c r="J5" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K5" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M5" s="17" t="s">
@@ -67968,12 +67973,12 @@
         <v>1583</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>1392</v>
       </c>
       <c r="B6" s="17" t="s">
@@ -67983,28 +67988,28 @@
         <v>1583</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>2034</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>2035</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>2036</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="12" t="s">
         <v>1583</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="50" t="s">
         <v>1278</v>
       </c>
-      <c r="J6" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K6" s="28" t="s">
+      <c r="J6" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K6" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M6" s="17" t="s">
@@ -68014,7 +68019,7 @@
         <v>1583</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -68030,7 +68035,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>1583</v>
@@ -68039,30 +68044,30 @@
         <v>1583</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>2037</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>2038</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>2039</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2040</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>2041</v>
-      </c>
-      <c r="J7" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K7" s="37" t="s">
+        <v>2040</v>
+      </c>
+      <c r="J7" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K7" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L7" s="37" t="s">
+      <c r="L7" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M7" s="17" t="s">
@@ -68072,13 +68077,13 @@
         <v>1583</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>1583</v>
@@ -68087,13 +68092,13 @@
         <v>1583</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>2042</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>2043</v>
       </c>
       <c r="G8" s="11">
         <v>988.0</v>
@@ -68102,15 +68107,15 @@
         <v>1583</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>2044</v>
-      </c>
-      <c r="J8" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K8" s="37" t="s">
+        <v>2043</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K8" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L8" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M8" s="17" t="s">
@@ -68120,13 +68125,13 @@
         <v>1583</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>1583</v>
@@ -68138,27 +68143,27 @@
         <v>1512</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>2044</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>2045</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>2046</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2047</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>2048</v>
-      </c>
-      <c r="J9" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K9" s="37" t="s">
+        <v>2047</v>
+      </c>
+      <c r="J9" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K9" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M9" s="17" t="s">
@@ -68168,13 +68173,13 @@
         <v>1583</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>1583</v>
@@ -68183,30 +68188,30 @@
         <v>1583</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>2048</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>2049</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>2050</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2051</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>2052</v>
-      </c>
-      <c r="J10" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K10" s="37" t="s">
+        <v>2051</v>
+      </c>
+      <c r="J10" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K10" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L10" s="37" t="s">
+      <c r="L10" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M10" s="17" t="s">
@@ -68216,13 +68221,13 @@
         <v>1583</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>1583</v>
@@ -68234,27 +68239,27 @@
         <v>1512</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>2053</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="3" t="s">
         <v>2054</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="27" t="s">
         <v>2055</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="I11" s="8" t="s">
         <v>2056</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>2057</v>
-      </c>
-      <c r="J11" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K11" s="37" t="s">
+      <c r="J11" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K11" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L11" s="37" t="s">
+      <c r="L11" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M11" s="17" t="s">
@@ -68264,7 +68269,7 @@
         <v>1583</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P11" s="2"/>
     </row>
@@ -68279,30 +68284,30 @@
         <v>1583</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>2057</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>2058</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>2059</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>2060</v>
-      </c>
-      <c r="J12" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K12" s="37" t="s">
+        <v>2059</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K12" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L12" s="37" t="s">
+      <c r="L12" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M12" s="17" t="s">
@@ -68312,7 +68317,7 @@
         <v>1583</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P12" s="2"/>
     </row>
@@ -68330,27 +68335,27 @@
         <v>1512</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>2060</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>2061</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="3" t="s">
         <v>2062</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>2063</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>2064</v>
-      </c>
-      <c r="J13" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K13" s="37" t="s">
+        <v>2063</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K13" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L13" s="37" t="s">
+      <c r="L13" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M13" s="17" t="s">
@@ -68360,7 +68365,7 @@
         <v>1583</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P13" s="2"/>
     </row>
@@ -68378,27 +68383,27 @@
         <v>1512</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>2064</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>2065</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="3" t="s">
         <v>2066</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2067</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>2068</v>
-      </c>
-      <c r="J14" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K14" s="28" t="s">
+        <v>2067</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K14" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="L14" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M14" s="17" t="s">
@@ -68408,7 +68413,7 @@
         <v>1583</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P14" s="2"/>
     </row>
@@ -68423,30 +68428,30 @@
         <v>1583</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>2068</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>2069</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="3" t="s">
         <v>2070</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>2071</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>2072</v>
-      </c>
-      <c r="J15" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K15" s="28" t="s">
+        <v>2071</v>
+      </c>
+      <c r="J15" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K15" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L15" s="28" t="s">
+      <c r="L15" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M15" s="17" t="s">
@@ -68456,7 +68461,7 @@
         <v>1583</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P15" s="2"/>
     </row>
@@ -68474,27 +68479,27 @@
         <v>1512</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>2072</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>2073</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="3" t="s">
         <v>2074</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>2075</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>2076</v>
-      </c>
-      <c r="J16" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K16" s="37" t="s">
+        <v>2075</v>
+      </c>
+      <c r="J16" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K16" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L16" s="37" t="s">
+      <c r="L16" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M16" s="17" t="s">
@@ -68504,7 +68509,7 @@
         <v>1583</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P16" s="2"/>
     </row>
@@ -68519,30 +68524,30 @@
         <v>1583</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>2076</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>2077</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="3" t="s">
         <v>2078</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>2079</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>2080</v>
-      </c>
-      <c r="J17" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K17" s="37" t="s">
+        <v>2079</v>
+      </c>
+      <c r="J17" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K17" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L17" s="37" t="s">
+      <c r="L17" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M17" s="17" t="s">
@@ -68552,7 +68557,7 @@
         <v>1583</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P17" s="2"/>
     </row>
@@ -68570,27 +68575,27 @@
         <v>1512</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>2080</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>2081</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="3" t="s">
         <v>2082</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>2083</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>2084</v>
-      </c>
-      <c r="J18" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K18" s="37" t="s">
+        <v>2083</v>
+      </c>
+      <c r="J18" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K18" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L18" s="37" t="s">
+      <c r="L18" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M18" s="17" t="s">
@@ -68600,7 +68605,7 @@
         <v>1583</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P18" s="2"/>
     </row>
@@ -68615,30 +68620,30 @@
         <v>1583</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>2084</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>2085</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="3" t="s">
         <v>2086</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>2087</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>2088</v>
-      </c>
-      <c r="J19" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K19" s="37" t="s">
+        <v>2087</v>
+      </c>
+      <c r="J19" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K19" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L19" s="37" t="s">
+      <c r="L19" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M19" s="17" t="s">
@@ -68648,7 +68653,7 @@
         <v>1583</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P19" s="2"/>
     </row>
@@ -68663,13 +68668,13 @@
         <v>1583</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>2088</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>2089</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>2090</v>
       </c>
       <c r="G20" s="11">
         <v>211.0</v>
@@ -68678,15 +68683,15 @@
         <v>1583</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>2091</v>
-      </c>
-      <c r="J20" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K20" s="37" t="s">
+        <v>2090</v>
+      </c>
+      <c r="J20" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K20" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L20" s="37" t="s">
+      <c r="L20" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M20" s="17" t="s">
@@ -68696,7 +68701,7 @@
         <v>1583</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P20" s="2"/>
     </row>
@@ -68711,13 +68716,13 @@
         <v>1583</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>2091</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>2092</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>2093</v>
       </c>
       <c r="G21" s="11">
         <v>988.0</v>
@@ -68726,15 +68731,15 @@
         <v>1583</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>2094</v>
-      </c>
-      <c r="J21" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K21" s="37" t="s">
+        <v>2093</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K21" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L21" s="37" t="s">
+      <c r="L21" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M21" s="17" t="s">
@@ -68744,7 +68749,7 @@
         <v>1583</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P21" s="2"/>
     </row>
@@ -68759,30 +68764,30 @@
         <v>1583</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>2094</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>2095</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="3" t="s">
         <v>2096</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>2097</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>2098</v>
-      </c>
-      <c r="J22" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K22" s="37" t="s">
+        <v>2097</v>
+      </c>
+      <c r="J22" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K22" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L22" s="37" t="s">
+      <c r="L22" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M22" s="17" t="s">
@@ -68792,7 +68797,7 @@
         <v>1583</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P22" s="2"/>
     </row>
@@ -68810,25 +68815,25 @@
         <v>1512</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>2098</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>2099</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>2100</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>2101</v>
-      </c>
-      <c r="J23" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K23" s="28" t="s">
+        <v>2100</v>
+      </c>
+      <c r="J23" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K23" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L23" s="28" t="s">
+      <c r="L23" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M23" s="17" t="s">
@@ -68838,7 +68843,7 @@
         <v>1583</v>
       </c>
       <c r="O23" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P23" s="2"/>
     </row>
@@ -68856,25 +68861,25 @@
         <v>1512</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>2101</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>2102</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>2103</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>2104</v>
-      </c>
-      <c r="J24" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K24" s="28" t="s">
+        <v>2103</v>
+      </c>
+      <c r="J24" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K24" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L24" s="28" t="s">
+      <c r="L24" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M24" s="17" t="s">
@@ -68884,7 +68889,7 @@
         <v>1583</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P24" s="2"/>
     </row>
@@ -68902,27 +68907,27 @@
         <v>1512</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>2104</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>2105</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="3" t="s">
         <v>2106</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>2107</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>1583</v>
       </c>
-      <c r="I25" s="34" t="s">
-        <v>2108</v>
-      </c>
-      <c r="J25" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K25" s="37" t="s">
+      <c r="I25" s="35" t="s">
+        <v>2107</v>
+      </c>
+      <c r="J25" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K25" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L25" s="37" t="s">
+      <c r="L25" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M25" s="17" t="s">
@@ -68932,7 +68937,7 @@
         <v>1583</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P25" s="2"/>
     </row>
@@ -68947,30 +68952,30 @@
         <v>1583</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>2108</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>2109</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>2110</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>1583</v>
       </c>
-      <c r="I26" s="48" t="s">
-        <v>2111</v>
-      </c>
-      <c r="J26" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K26" s="37" t="s">
+      <c r="I26" s="50" t="s">
+        <v>2110</v>
+      </c>
+      <c r="J26" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K26" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L26" s="37" t="s">
+      <c r="L26" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M26" s="17" t="s">
@@ -68980,7 +68985,7 @@
         <v>1583</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P26" s="2"/>
     </row>
@@ -68998,27 +69003,27 @@
         <v>1535</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>2111</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>2112</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="3" t="s">
         <v>2113</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>2114</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>2115</v>
-      </c>
-      <c r="J27" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K27" s="37" t="s">
+        <v>2114</v>
+      </c>
+      <c r="J27" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K27" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L27" s="37" t="s">
+      <c r="L27" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M27" s="17" t="s">
@@ -69028,7 +69033,7 @@
         <v>1583</v>
       </c>
       <c r="O27" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P27" s="2"/>
     </row>
@@ -69046,10 +69051,10 @@
         <v>1512</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>2115</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>2116</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>2117</v>
       </c>
       <c r="G28" s="11">
         <v>811.0</v>
@@ -69058,15 +69063,15 @@
         <v>1583</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>2118</v>
-      </c>
-      <c r="J28" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K28" s="37" t="s">
+        <v>2117</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K28" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L28" s="37" t="s">
+      <c r="L28" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M28" s="17" t="s">
@@ -69076,7 +69081,7 @@
         <v>1583</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P28" s="2"/>
     </row>
@@ -69094,27 +69099,27 @@
         <v>1738</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>2118</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>2119</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="3" t="s">
         <v>2120</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>2121</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>2122</v>
-      </c>
-      <c r="J29" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K29" s="37" t="s">
+        <v>2121</v>
+      </c>
+      <c r="J29" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K29" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L29" s="37" t="s">
+      <c r="L29" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M29" s="17" t="s">
@@ -69124,7 +69129,7 @@
         <v>1583</v>
       </c>
       <c r="O29" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P29" s="2"/>
     </row>
@@ -69139,30 +69144,30 @@
         <v>1583</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>2122</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>2123</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="3" t="s">
         <v>2124</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>2125</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>2126</v>
-      </c>
-      <c r="J30" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K30" s="37" t="s">
+        <v>2125</v>
+      </c>
+      <c r="J30" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K30" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L30" s="37" t="s">
+      <c r="L30" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M30" s="17" t="s">
@@ -69172,7 +69177,7 @@
         <v>1583</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P30" s="2"/>
     </row>
@@ -69190,10 +69195,10 @@
         <v>1512</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>2126</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>2127</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>2128</v>
       </c>
       <c r="G31" s="11">
         <v>811.0</v>
@@ -69202,15 +69207,15 @@
         <v>1583</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>2129</v>
-      </c>
-      <c r="J31" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K31" s="37" t="s">
+        <v>2128</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K31" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L31" s="37" t="s">
+      <c r="L31" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M31" s="17" t="s">
@@ -69220,7 +69225,7 @@
         <v>1583</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P31" s="2"/>
     </row>
@@ -69238,25 +69243,25 @@
         <v>1512</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>2129</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>2130</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>2131</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>2132</v>
-      </c>
-      <c r="J32" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K32" s="28" t="s">
+        <v>2131</v>
+      </c>
+      <c r="J32" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K32" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L32" s="28" t="s">
+      <c r="L32" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M32" s="17" t="s">
@@ -69266,7 +69271,7 @@
         <v>1583</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P32" s="2"/>
     </row>
@@ -69284,27 +69289,27 @@
         <v>1512</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>2132</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>2133</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="3" t="s">
         <v>2134</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>2135</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>2136</v>
-      </c>
-      <c r="J33" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K33" s="28" t="s">
+        <v>2135</v>
+      </c>
+      <c r="J33" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K33" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L33" s="28" t="s">
+      <c r="L33" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M33" s="17" t="s">
@@ -69314,13 +69319,13 @@
         <v>1583</v>
       </c>
       <c r="O33" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P33" s="2"/>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>1583</v>
@@ -69329,30 +69334,30 @@
         <v>1583</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>2137</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>2138</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="3" t="s">
         <v>2139</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>2140</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>2141</v>
-      </c>
-      <c r="J34" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K34" s="37" t="s">
+        <v>2140</v>
+      </c>
+      <c r="J34" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K34" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L34" s="37" t="s">
+      <c r="L34" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M34" s="17" t="s">
@@ -69362,7 +69367,7 @@
         <v>1583</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P34" s="2"/>
     </row>
@@ -69377,28 +69382,28 @@
         <v>1583</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E35" s="3" t="s">
+        <v>2141</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>2142</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>2143</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>2144</v>
-      </c>
-      <c r="J35" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K35" s="37" t="s">
+        <v>2143</v>
+      </c>
+      <c r="J35" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K35" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L35" s="37" t="s">
+      <c r="L35" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M35" s="17" t="s">
@@ -69408,7 +69413,7 @@
         <v>1583</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P35" s="2"/>
     </row>
@@ -69423,30 +69428,30 @@
         <v>1583</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>1583</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>2146</v>
-      </c>
-      <c r="J36" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K36" s="37" t="s">
+        <v>2145</v>
+      </c>
+      <c r="J36" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K36" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L36" s="37" t="s">
+      <c r="L36" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M36" s="17" t="s">
@@ -69456,13 +69461,13 @@
         <v>1583</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P36" s="2"/>
     </row>
     <row r="37">
       <c r="A37" s="17" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>1583</v>
@@ -69474,25 +69479,25 @@
         <v>1738</v>
       </c>
       <c r="E37" s="17" t="s">
+        <v>2147</v>
+      </c>
+      <c r="F37" s="17" t="s">
         <v>2148</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="G37" s="2"/>
+      <c r="H37" s="30" t="s">
         <v>2149</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="29" t="s">
+      <c r="I37" s="31" t="s">
         <v>2150</v>
       </c>
-      <c r="I37" s="30" t="s">
-        <v>2151</v>
-      </c>
-      <c r="J37" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K37" s="28" t="s">
+      <c r="J37" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K37" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L37" s="28" t="s">
+      <c r="L37" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M37" s="17" t="s">
@@ -69502,13 +69507,13 @@
         <v>1583</v>
       </c>
       <c r="O37" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P37" s="2"/>
     </row>
     <row r="38">
       <c r="A38" s="17" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>1583</v>
@@ -69519,26 +69524,26 @@
       <c r="D38" s="10" t="s">
         <v>1503</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="29" t="s">
+        <v>2151</v>
+      </c>
+      <c r="F38" s="29" t="s">
         <v>2152</v>
       </c>
-      <c r="F38" s="28" t="s">
+      <c r="G38" s="2"/>
+      <c r="H38" s="30" t="s">
         <v>2153</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="29" t="s">
+      <c r="I38" s="31" t="s">
         <v>2154</v>
       </c>
-      <c r="I38" s="30" t="s">
-        <v>2155</v>
-      </c>
-      <c r="J38" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K38" s="28" t="s">
+      <c r="J38" s="48" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K38" s="29" t="s">
         <v>1510</v>
       </c>
-      <c r="L38" s="28" t="s">
+      <c r="L38" s="29" t="s">
         <v>1510</v>
       </c>
       <c r="M38" s="17" t="s">
@@ -69548,13 +69553,13 @@
         <v>1583</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P38" s="2"/>
     </row>
     <row r="39">
       <c r="A39" s="17" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>1583</v>
@@ -69563,30 +69568,30 @@
         <v>1583</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E39" s="5" t="s">
+        <v>2155</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>2156</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="G39" s="5" t="s">
         <v>2157</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="30" t="s">
+        <v>1583</v>
+      </c>
+      <c r="I39" s="21" t="s">
         <v>2158</v>
       </c>
-      <c r="H39" s="29" t="s">
-        <v>1583</v>
-      </c>
-      <c r="I39" s="21" t="s">
+      <c r="J39" s="5" t="s">
         <v>2159</v>
       </c>
-      <c r="J39" s="5" t="s">
-        <v>2160</v>
-      </c>
-      <c r="K39" s="37" t="s">
+      <c r="K39" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L39" s="37" t="s">
+      <c r="L39" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M39" s="17" t="s">
@@ -69596,7 +69601,7 @@
         <v>1583</v>
       </c>
       <c r="O39" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
@@ -69621,30 +69626,30 @@
         <v>1583</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E40" s="5" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>2161</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="G40" s="5" t="s">
         <v>2162</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="H40" s="30" t="s">
+        <v>1583</v>
+      </c>
+      <c r="I40" s="21" t="s">
         <v>2163</v>
       </c>
-      <c r="H40" s="29" t="s">
-        <v>1583</v>
-      </c>
-      <c r="I40" s="21" t="s">
+      <c r="J40" s="5" t="s">
         <v>2164</v>
       </c>
-      <c r="J40" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K40" s="37" t="s">
+      <c r="K40" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L40" s="37" t="s">
+      <c r="L40" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M40" s="17" t="s">
@@ -69654,7 +69659,7 @@
         <v>1583</v>
       </c>
       <c r="O40" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
@@ -69670,7 +69675,7 @@
     </row>
     <row r="41">
       <c r="A41" s="17" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>1583</v>
@@ -69690,19 +69695,19 @@
       <c r="G41" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="H41" s="30" t="s">
+      <c r="H41" s="31" t="s">
         <v>2167</v>
       </c>
-      <c r="I41" s="31" t="s">
+      <c r="I41" s="32" t="s">
         <v>2168</v>
       </c>
-      <c r="J41" s="49">
-        <v>45862.0</v>
-      </c>
-      <c r="K41" s="37" t="s">
+      <c r="J41" s="46" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K41" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L41" s="37" t="s">
+      <c r="L41" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M41" s="17" t="s">
@@ -69712,7 +69717,7 @@
         <v>1583</v>
       </c>
       <c r="O41" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
@@ -69728,7 +69733,7 @@
     </row>
     <row r="42">
       <c r="A42" s="17" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B42" s="17" t="s">
         <v>1583</v>
@@ -69748,19 +69753,19 @@
       <c r="G42" s="17" t="s">
         <v>2171</v>
       </c>
-      <c r="H42" s="29" t="s">
+      <c r="H42" s="30" t="s">
         <v>1583</v>
       </c>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="32" t="s">
         <v>2172</v>
       </c>
       <c r="J42" s="17" t="s">
         <v>2173</v>
       </c>
-      <c r="K42" s="37" t="s">
+      <c r="K42" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L42" s="37" t="s">
+      <c r="L42" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M42" s="17" t="s">
@@ -69770,7 +69775,7 @@
         <v>1583</v>
       </c>
       <c r="O42" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
@@ -69795,7 +69800,7 @@
         <v>1583</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E43" s="17" t="s">
         <v>2174</v>
@@ -69806,19 +69811,19 @@
       <c r="G43" s="17" t="s">
         <v>2176</v>
       </c>
-      <c r="H43" s="29" t="s">
+      <c r="H43" s="30" t="s">
         <v>1583</v>
       </c>
-      <c r="I43" s="31" t="s">
+      <c r="I43" s="32" t="s">
         <v>2177</v>
       </c>
-      <c r="J43" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K43" s="37" t="s">
+      <c r="J43" s="28" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K43" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L43" s="37" t="s">
+      <c r="L43" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M43" s="17" t="s">
@@ -69828,7 +69833,7 @@
         <v>1583</v>
       </c>
       <c r="O43" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="44">
@@ -69842,7 +69847,7 @@
         <v>1583</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>2178</v>
@@ -69853,19 +69858,19 @@
       <c r="G44" s="17" t="s">
         <v>1583</v>
       </c>
-      <c r="H44" s="29" t="s">
+      <c r="H44" s="30" t="s">
         <v>1583</v>
       </c>
-      <c r="I44" s="31" t="s">
+      <c r="I44" s="32" t="s">
         <v>2180</v>
       </c>
-      <c r="J44" s="49">
-        <v>45862.0</v>
-      </c>
-      <c r="K44" s="37" t="s">
+      <c r="J44" s="46" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K44" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L44" s="37" t="s">
+      <c r="L44" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M44" s="17" t="s">
@@ -69875,12 +69880,12 @@
         <v>1583</v>
       </c>
       <c r="O44" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="17" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>1583</v>
@@ -69900,19 +69905,19 @@
       <c r="G45" s="5" t="s">
         <v>2182</v>
       </c>
-      <c r="H45" s="29" t="s">
+      <c r="H45" s="30" t="s">
         <v>2183</v>
       </c>
       <c r="I45" s="20" t="s">
         <v>2184</v>
       </c>
-      <c r="J45" s="41" t="s">
+      <c r="J45" s="42" t="s">
         <v>2185</v>
       </c>
-      <c r="K45" s="37" t="s">
+      <c r="K45" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L45" s="37" t="s">
+      <c r="L45" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M45" s="17" t="s">
@@ -69922,12 +69927,12 @@
         <v>1583</v>
       </c>
       <c r="O45" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="17" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>1583</v>
@@ -69947,19 +69952,19 @@
       <c r="G46" s="17" t="s">
         <v>2187</v>
       </c>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="30" t="s">
         <v>2188</v>
       </c>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="32" t="s">
         <v>2189</v>
       </c>
-      <c r="J46" s="47">
-        <v>45862.0</v>
-      </c>
-      <c r="K46" s="37" t="s">
+      <c r="J46" s="28" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K46" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L46" s="37" t="s">
+      <c r="L46" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M46" s="17" t="s">
@@ -69969,7 +69974,7 @@
         <v>1583</v>
       </c>
       <c r="O46" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="47">
@@ -69994,19 +69999,19 @@
       <c r="G47" s="17" t="s">
         <v>2192</v>
       </c>
-      <c r="H47" s="30" t="s">
+      <c r="H47" s="31" t="s">
         <v>2193</v>
       </c>
-      <c r="I47" s="31" t="s">
+      <c r="I47" s="32" t="s">
         <v>2194</v>
       </c>
       <c r="J47" s="17" t="s">
         <v>2195</v>
       </c>
-      <c r="K47" s="37" t="s">
+      <c r="K47" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L47" s="37" t="s">
+      <c r="L47" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M47" s="17" t="s">
@@ -70016,12 +70021,12 @@
         <v>1583</v>
       </c>
       <c r="O47" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="17" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>1583</v>
@@ -70044,16 +70049,16 @@
       <c r="H48" s="12" t="s">
         <v>1583</v>
       </c>
-      <c r="I48" s="30" t="s">
+      <c r="I48" s="31" t="s">
         <v>2199</v>
       </c>
-      <c r="J48" s="49">
-        <v>45862.0</v>
-      </c>
-      <c r="K48" s="37" t="s">
+      <c r="J48" s="46" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K48" s="38" t="s">
         <v>1510</v>
       </c>
-      <c r="L48" s="37" t="s">
+      <c r="L48" s="38" t="s">
         <v>1510</v>
       </c>
       <c r="M48" s="17" t="s">
@@ -70063,7 +70068,7 @@
         <v>1583</v>
       </c>
       <c r="O48" s="10" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>